<commit_message>
updated details to project
</commit_message>
<xml_diff>
--- a/Salesforce/src/main/java/resources/DataSource.xlsx
+++ b/Salesforce/src/main/java/resources/DataSource.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -39,13 +39,7 @@
     <t>SearchText</t>
   </si>
   <si>
-    <t>Fortis</t>
-  </si>
-  <si>
-    <t>ati</t>
-  </si>
-  <si>
-    <t>Ash</t>
+    <t>Gary Abbott</t>
   </si>
 </sst>
 </file>
@@ -419,10 +413,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -435,16 +429,6 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>